<commit_message>
chore: update testbench results
</commit_message>
<xml_diff>
--- a/docs/uart_report.xlsx
+++ b/docs/uart_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UF523TCH\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126DA8DC-CF7A-4B2A-A37E-051B83F32961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0BB104-322C-49A6-8B39-0F4811EEA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{85EF69C1-0CF4-4C88-A077-43C70A228E3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{85EF69C1-0CF4-4C88-A077-43C70A228E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="coverage" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="787">
   <si>
     <t>#-----------------------------------------------------------</t>
   </si>
@@ -1457,27 +1457,7 @@
   </si>
   <si>
     <t xml:space="preserve">Signal assignment statement:
-259:                next_state &lt;= STATE_IDLE; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signal assignment statement:
-309:                next_tx_data   &lt;= (others =&gt; '0'); </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signal assignment statement:
-310:                next_o_uart_tx &lt;= '1'; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signal assignment statement:
 311:                next_o_done    &lt;= '0'; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"case" / "with" / "select" choice:
-257:            when others =&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"case" / "with" / "select" choice:
-307:            when others =&gt; </t>
   </si>
   <si>
     <t>INST_UART_RX</t>
@@ -2496,6 +2476,30 @@
       </rPr>
       <t>: Vivado skipped parallel synthesis because the design is too small to benefit from multi-threading, which affects only compilation time, not hardware functionality or performance. Read more here: https://stackoverflow.com/questions/79563001/vivado-2024-1-warning-synth-8-7080-parallel-synthesis-criteria-is-not-met</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal assignment statement:
+261:                next_state &lt;= STATE_IDLE; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal assignment statement:
+311:                next_tx_data   &lt;= (others =&gt; '0'); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal assignment statement:
+312:                next_o_uart_tx &lt;= '1'; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal assignment statement:
+313:                next_o_done    &lt;= '0'; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"case" / "with" / "select" choice:
+259:            when others =&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"case" / "with" / "select" choice:
+309:            when others =&gt; </t>
   </si>
 </sst>
 </file>
@@ -2777,7 +2781,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2796,24 +2814,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2823,10 +2823,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3219,10 +3223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18D19E-3FCF-405F-85CF-7C7CF68FC2BB}">
-  <dimension ref="B2:M41"/>
+  <dimension ref="B2:M42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:G21"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,14 +3238,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="5" t="s">
         <v>456</v>
       </c>
@@ -3262,16 +3266,16 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="2">
-        <v>0.97</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="I3" s="2">
         <v>0.95699999999999996</v>
@@ -3289,13 +3293,13 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="2">
         <v>1</v>
       </c>
@@ -3313,13 +3317,13 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="2">
         <v>0.96599999999999997</v>
       </c>
@@ -3339,175 +3343,175 @@
     </row>
     <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="20" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="22"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="7" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="20" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="22"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="7" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="20" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="14"/>
       <c r="M8" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="20" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="22"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="14"/>
       <c r="M9" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="20" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="22"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="7" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="20" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="22"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
       <c r="M11" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="20" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
       <c r="M12" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="20" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="12" t="s">
         <v>467</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="22"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
       <c r="M13" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="20" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="22"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="14"/>
       <c r="M14" s="7" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="2">
         <v>0.94499999999999995</v>
       </c>
@@ -3528,318 +3532,322 @@
     <row r="16" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16"/>
       <c r="C16"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="20" t="s">
-        <v>470</v>
-      </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="22"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="12" t="s">
+        <v>781</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
       <c r="M16" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17"/>
       <c r="C17"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="22"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="12" t="s">
+        <v>782</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
       <c r="M17" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="22"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="12" t="s">
+        <v>783</v>
+      </c>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="14"/>
       <c r="M18" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="22"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="14"/>
       <c r="M19" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="20" t="s">
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="12" t="s">
+        <v>784</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="7" t="s">
         <v>474</v>
-      </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="7" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="22"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="12" t="s">
+        <v>785</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="14"/>
       <c r="M21" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22" s="11" t="s">
-        <v>476</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1</v>
-      </c>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="20" t="s">
-        <v>481</v>
-      </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="7" t="s">
-        <v>479</v>
-      </c>
+      <c r="D23" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="20" t="s">
-        <v>482</v>
-      </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="22"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="14"/>
       <c r="M24" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="20" t="s">
-        <v>483</v>
-      </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="22"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="14"/>
       <c r="M25" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="20" t="s">
-        <v>484</v>
-      </c>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="22"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="14"/>
       <c r="M26" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="22"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="14"/>
       <c r="M27" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="20" t="s">
-        <v>486</v>
-      </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="22"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="14"/>
       <c r="M28" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="29" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="20" t="s">
-        <v>487</v>
-      </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="22"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="14"/>
       <c r="M29" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="20" t="s">
-        <v>488</v>
-      </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="22"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="14"/>
       <c r="M30" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31"/>
-      <c r="C31" s="17" t="s">
-        <v>477</v>
-      </c>
+      <c r="C31"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1</v>
-      </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="6"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="7" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32"/>
+      <c r="C32" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="6"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33"/>
@@ -3848,11 +3856,11 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
       <c r="M33"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
@@ -3862,11 +3870,11 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
       <c r="M34"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -3876,11 +3884,11 @@
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
       <c r="M35"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
@@ -3890,11 +3898,11 @@
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
       <c r="M36"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -3904,11 +3912,11 @@
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
       <c r="M37"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
@@ -3918,11 +3926,11 @@
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
       <c r="M38"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -3932,11 +3940,11 @@
       <c r="E39"/>
       <c r="F39"/>
       <c r="G39"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
       <c r="M39"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
@@ -3946,11 +3954,11 @@
       <c r="E40"/>
       <c r="F40"/>
       <c r="G40"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
       <c r="M40"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
@@ -3960,20 +3968,53 @@
       <c r="E41"/>
       <c r="F41"/>
       <c r="G41"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
       <c r="M41"/>
     </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="H7:L7"/>
+  <mergeCells count="41">
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="D23:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="H21:L21"/>
     <mergeCell ref="H14:L14"/>
     <mergeCell ref="C5:G14"/>
     <mergeCell ref="H16:L16"/>
@@ -3985,38 +4026,20 @@
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D15:G21"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="H24:L24"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="D22:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="D15:G22"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="H7:L7"/>
   </mergeCells>
-  <conditionalFormatting sqref="H32:H41">
+  <conditionalFormatting sqref="H33:H42">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>98%</formula>
       <formula>100%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:L31">
+  <conditionalFormatting sqref="H3:L32">
     <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
       <formula>99.99%</formula>
       <formula>100%</formula>
@@ -4125,7 +4148,7 @@
         <v/>
       </c>
       <c r="C8" s="4" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -4135,7 +4158,7 @@
         <v/>
       </c>
       <c r="C9" s="4" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -4285,7 +4308,7 @@
         <v/>
       </c>
       <c r="C24" s="4" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="D24" s="4"/>
     </row>
@@ -4495,7 +4518,7 @@
         <v/>
       </c>
       <c r="C45" s="4" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D45" s="4"/>
     </row>
@@ -4505,7 +4528,7 @@
         <v/>
       </c>
       <c r="C46" s="4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D46" s="4"/>
     </row>
@@ -4515,7 +4538,7 @@
         <v/>
       </c>
       <c r="C47" s="4" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D47" s="4"/>
     </row>
@@ -4525,7 +4548,7 @@
         <v/>
       </c>
       <c r="C48" s="4" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D48" s="4"/>
     </row>
@@ -4535,7 +4558,7 @@
         <v/>
       </c>
       <c r="C49" s="4" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D49" s="4"/>
     </row>
@@ -4545,7 +4568,7 @@
         <v/>
       </c>
       <c r="C50" s="4" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D50" s="4"/>
     </row>
@@ -4555,7 +4578,7 @@
         <v/>
       </c>
       <c r="C51" s="4" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D51" s="4"/>
     </row>
@@ -4595,7 +4618,7 @@
         <v/>
       </c>
       <c r="C55" s="4" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D55" s="4"/>
     </row>
@@ -4655,7 +4678,7 @@
         <v/>
       </c>
       <c r="C61" s="4" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D61" s="4"/>
     </row>
@@ -4685,7 +4708,7 @@
         <v/>
       </c>
       <c r="C64" s="4" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D64" s="4"/>
     </row>
@@ -4975,7 +4998,7 @@
         <v>INFO</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D93" s="4"/>
     </row>
@@ -4995,7 +5018,7 @@
         <v/>
       </c>
       <c r="C95" s="4" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D95" s="4"/>
     </row>
@@ -5015,7 +5038,7 @@
         <v>INFO</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D97" s="4"/>
     </row>
@@ -5025,7 +5048,7 @@
         <v/>
       </c>
       <c r="C98" s="4" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D98" s="4"/>
     </row>
@@ -5035,7 +5058,7 @@
         <v>INFO</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D99" s="4"/>
     </row>
@@ -5045,7 +5068,7 @@
         <v/>
       </c>
       <c r="C100" s="4" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D100" s="4"/>
     </row>
@@ -5055,7 +5078,7 @@
         <v/>
       </c>
       <c r="C101" s="4" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D101" s="4"/>
     </row>
@@ -5065,7 +5088,7 @@
         <v>INFO</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D102" s="4"/>
     </row>
@@ -5075,7 +5098,7 @@
         <v>INFO</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D103" s="4"/>
     </row>
@@ -5085,7 +5108,7 @@
         <v/>
       </c>
       <c r="C104" s="4" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D104" s="4"/>
     </row>
@@ -5095,7 +5118,7 @@
         <v/>
       </c>
       <c r="C105" s="4" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D105" s="4"/>
     </row>
@@ -5105,7 +5128,7 @@
         <v/>
       </c>
       <c r="C106" s="4" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D106" s="4"/>
     </row>
@@ -5115,7 +5138,7 @@
         <v>INFO</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D107" s="4"/>
     </row>
@@ -5125,7 +5148,7 @@
         <v/>
       </c>
       <c r="C108" s="4" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D108" s="4"/>
     </row>
@@ -5135,7 +5158,7 @@
         <v/>
       </c>
       <c r="C109" s="4" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D109" s="4"/>
     </row>
@@ -5145,7 +5168,7 @@
         <v>INFO</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D110" s="4"/>
     </row>
@@ -5155,7 +5178,7 @@
         <v>INFO</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D111" s="4"/>
     </row>
@@ -5165,7 +5188,7 @@
         <v/>
       </c>
       <c r="C112" s="4" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D112" s="4"/>
     </row>
@@ -5175,7 +5198,7 @@
         <v/>
       </c>
       <c r="C113" s="4" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D113" s="4"/>
     </row>
@@ -5185,7 +5208,7 @@
         <v/>
       </c>
       <c r="C114" s="4" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D114" s="4"/>
     </row>
@@ -5195,7 +5218,7 @@
         <v>INFO</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D115" s="4"/>
     </row>
@@ -5205,7 +5228,7 @@
         <v>INFO</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="D116" s="4"/>
     </row>
@@ -5215,7 +5238,7 @@
         <v>INFO</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D117" s="4"/>
     </row>
@@ -5225,7 +5248,7 @@
         <v>INFO</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="D118" s="4"/>
     </row>
@@ -5235,7 +5258,7 @@
         <v>INFO</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="D119" s="4"/>
     </row>
@@ -5245,7 +5268,7 @@
         <v>INFO</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="D120" s="4"/>
     </row>
@@ -5255,7 +5278,7 @@
         <v/>
       </c>
       <c r="C121" s="4" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D121" s="4"/>
     </row>
@@ -5265,7 +5288,7 @@
         <v/>
       </c>
       <c r="C122" s="4" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D122" s="4"/>
     </row>
@@ -5275,7 +5298,7 @@
         <v>INFO</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="D123" s="4"/>
     </row>
@@ -5285,7 +5308,7 @@
         <v>INFO</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="D124" s="4"/>
     </row>
@@ -5305,7 +5328,7 @@
         <v/>
       </c>
       <c r="C126" s="4" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="D126" s="4"/>
     </row>
@@ -5365,7 +5388,7 @@
         <v/>
       </c>
       <c r="C132" s="4" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="D132" s="4"/>
     </row>
@@ -5395,7 +5418,7 @@
         <v/>
       </c>
       <c r="C135" s="4" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D135" s="4"/>
     </row>
@@ -5415,7 +5438,7 @@
         <v/>
       </c>
       <c r="C137" s="4" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="D137" s="4"/>
     </row>
@@ -5541,7 +5564,7 @@
         <v/>
       </c>
       <c r="C150" s="4" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D150" s="4"/>
     </row>
@@ -5579,7 +5602,7 @@
         <v/>
       </c>
       <c r="C154" s="4" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D154" s="4"/>
     </row>
@@ -5599,7 +5622,7 @@
         <v/>
       </c>
       <c r="C156" s="4" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="D156" s="4"/>
     </row>
@@ -5669,7 +5692,7 @@
         <v/>
       </c>
       <c r="C163" s="4" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D163" s="4"/>
     </row>
@@ -5729,7 +5752,7 @@
         <v/>
       </c>
       <c r="C169" s="4" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D169" s="4"/>
     </row>
@@ -5789,7 +5812,7 @@
         <v/>
       </c>
       <c r="C175" s="4" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="D175" s="4"/>
     </row>
@@ -5809,7 +5832,7 @@
         <v/>
       </c>
       <c r="C177" s="4" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D177" s="4"/>
     </row>
@@ -5819,7 +5842,7 @@
         <v/>
       </c>
       <c r="C178" s="4" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="D178" s="4"/>
     </row>
@@ -5829,7 +5852,7 @@
         <v/>
       </c>
       <c r="C179" s="4" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D179" s="4"/>
     </row>
@@ -5849,7 +5872,7 @@
         <v>INFO</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D181" s="4"/>
     </row>
@@ -5869,7 +5892,7 @@
         <v/>
       </c>
       <c r="C183" s="4" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="D183" s="4"/>
     </row>
@@ -5989,7 +6012,7 @@
         <v/>
       </c>
       <c r="C195" s="4" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="D195" s="4"/>
     </row>
@@ -6119,7 +6142,7 @@
         <v/>
       </c>
       <c r="C208" s="4" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="D208" s="4"/>
     </row>
@@ -6149,7 +6172,7 @@
         <v/>
       </c>
       <c r="C211" s="4" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="D211" s="4"/>
     </row>
@@ -6169,7 +6192,7 @@
         <v/>
       </c>
       <c r="C213" s="4" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="D213" s="4"/>
     </row>
@@ -6179,7 +6202,7 @@
         <v/>
       </c>
       <c r="C214" s="4" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D214" s="4"/>
     </row>
@@ -6189,7 +6212,7 @@
         <v/>
       </c>
       <c r="C215" s="4" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="D215" s="4"/>
     </row>
@@ -6199,7 +6222,7 @@
         <v/>
       </c>
       <c r="C216" s="4" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D216" s="4"/>
     </row>
@@ -6209,7 +6232,7 @@
         <v/>
       </c>
       <c r="C217" s="4" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D217" s="4"/>
     </row>
@@ -6219,7 +6242,7 @@
         <v/>
       </c>
       <c r="C218" s="4" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D218" s="4"/>
     </row>
@@ -6229,7 +6252,7 @@
         <v/>
       </c>
       <c r="C219" s="4" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="D219" s="4"/>
     </row>
@@ -6239,7 +6262,7 @@
         <v/>
       </c>
       <c r="C220" s="4" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D220" s="4"/>
     </row>
@@ -6249,7 +6272,7 @@
         <v/>
       </c>
       <c r="C221" s="4" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="D221" s="4"/>
     </row>
@@ -6259,7 +6282,7 @@
         <v/>
       </c>
       <c r="C222" s="4" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D222" s="4"/>
     </row>
@@ -6269,7 +6292,7 @@
         <v/>
       </c>
       <c r="C223" s="4" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="D223" s="4"/>
     </row>
@@ -6279,7 +6302,7 @@
         <v/>
       </c>
       <c r="C224" s="4" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D224" s="4"/>
     </row>
@@ -6289,7 +6312,7 @@
         <v/>
       </c>
       <c r="C225" s="4" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="D225" s="4"/>
     </row>
@@ -6299,7 +6322,7 @@
         <v/>
       </c>
       <c r="C226" s="4" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D226" s="4"/>
     </row>
@@ -6309,7 +6332,7 @@
         <v/>
       </c>
       <c r="C227" s="4" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="D227" s="4"/>
     </row>
@@ -6319,7 +6342,7 @@
         <v/>
       </c>
       <c r="C228" s="4" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="D228" s="4"/>
     </row>
@@ -6329,7 +6352,7 @@
         <v/>
       </c>
       <c r="C229" s="4" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="D229" s="4"/>
     </row>
@@ -6339,7 +6362,7 @@
         <v/>
       </c>
       <c r="C230" s="4" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="D230" s="4"/>
     </row>
@@ -6349,7 +6372,7 @@
         <v/>
       </c>
       <c r="C231" s="4" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D231" s="4"/>
     </row>
@@ -6359,7 +6382,7 @@
         <v/>
       </c>
       <c r="C232" s="4" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="D232" s="4"/>
     </row>
@@ -6369,7 +6392,7 @@
         <v/>
       </c>
       <c r="C233" s="4" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D233" s="4"/>
     </row>
@@ -6379,7 +6402,7 @@
         <v/>
       </c>
       <c r="C234" s="4" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D234" s="4"/>
     </row>
@@ -6389,7 +6412,7 @@
         <v/>
       </c>
       <c r="C235" s="4" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D235" s="4"/>
     </row>
@@ -6399,7 +6422,7 @@
         <v/>
       </c>
       <c r="C236" s="4" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="D236" s="4"/>
     </row>
@@ -6409,7 +6432,7 @@
         <v/>
       </c>
       <c r="C237" s="4" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D237" s="4"/>
     </row>
@@ -6419,7 +6442,7 @@
         <v/>
       </c>
       <c r="C238" s="4" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D238" s="4"/>
     </row>
@@ -6429,7 +6452,7 @@
         <v/>
       </c>
       <c r="C239" s="4" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D239" s="4"/>
     </row>
@@ -6439,7 +6462,7 @@
         <v/>
       </c>
       <c r="C240" s="4" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="D240" s="4"/>
     </row>
@@ -6449,7 +6472,7 @@
         <v/>
       </c>
       <c r="C241" s="4" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D241" s="4"/>
     </row>
@@ -6459,7 +6482,7 @@
         <v/>
       </c>
       <c r="C242" s="4" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="D242" s="4"/>
     </row>
@@ -6469,7 +6492,7 @@
         <v/>
       </c>
       <c r="C243" s="4" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="D243" s="4"/>
     </row>
@@ -6479,7 +6502,7 @@
         <v/>
       </c>
       <c r="C244" s="4" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="D244" s="4"/>
     </row>
@@ -6489,7 +6512,7 @@
         <v/>
       </c>
       <c r="C245" s="4" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="D245" s="4"/>
     </row>
@@ -6499,7 +6522,7 @@
         <v/>
       </c>
       <c r="C246" s="4" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D246" s="4"/>
     </row>
@@ -6509,7 +6532,7 @@
         <v/>
       </c>
       <c r="C247" s="4" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="D247" s="4"/>
     </row>
@@ -6529,7 +6552,7 @@
         <v/>
       </c>
       <c r="C249" s="4" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D249" s="4"/>
     </row>
@@ -6672,7 +6695,7 @@
         <v>118</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
     </row>
     <row r="264" spans="2:4" x14ac:dyDescent="0.25">
@@ -6691,7 +6714,7 @@
         <v/>
       </c>
       <c r="C265" s="4" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="D265" s="4"/>
     </row>
@@ -6751,7 +6774,7 @@
         <v/>
       </c>
       <c r="C271" s="4" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="D271" s="4"/>
     </row>
@@ -6811,7 +6834,7 @@
         <v/>
       </c>
       <c r="C277" s="4" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D277" s="4"/>
     </row>
@@ -6871,7 +6894,7 @@
         <v/>
       </c>
       <c r="C283" s="4" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D283" s="4"/>
     </row>
@@ -7051,7 +7074,7 @@
         <v/>
       </c>
       <c r="C301" s="4" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="D301" s="4"/>
     </row>
@@ -7111,7 +7134,7 @@
         <v/>
       </c>
       <c r="C307" s="4" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="D307" s="4"/>
     </row>
@@ -7171,7 +7194,7 @@
         <v/>
       </c>
       <c r="C313" s="4" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="D313" s="4"/>
     </row>
@@ -7231,7 +7254,7 @@
         <v/>
       </c>
       <c r="C319" s="4" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="D319" s="4"/>
     </row>
@@ -7291,7 +7314,7 @@
         <v/>
       </c>
       <c r="C325" s="4" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="D325" s="4"/>
     </row>
@@ -7351,7 +7374,7 @@
         <v/>
       </c>
       <c r="C331" s="4" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="D331" s="4"/>
     </row>
@@ -7409,7 +7432,7 @@
         <v/>
       </c>
       <c r="C337" s="4" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="D337" s="4"/>
     </row>
@@ -7467,7 +7490,7 @@
         <v/>
       </c>
       <c r="C343" s="4" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="D343" s="4"/>
     </row>
@@ -7477,7 +7500,7 @@
         <v/>
       </c>
       <c r="C344" s="4" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D344" s="4"/>
     </row>
@@ -7487,7 +7510,7 @@
         <v/>
       </c>
       <c r="C345" s="4" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="D345" s="4"/>
     </row>
@@ -7497,7 +7520,7 @@
         <v/>
       </c>
       <c r="C346" s="4" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D346" s="4"/>
     </row>
@@ -7507,7 +7530,7 @@
         <v/>
       </c>
       <c r="C347" s="4" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="D347" s="4"/>
     </row>
@@ -7517,7 +7540,7 @@
         <v/>
       </c>
       <c r="C348" s="4" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="D348" s="4"/>
     </row>
@@ -7527,7 +7550,7 @@
         <v/>
       </c>
       <c r="C349" s="4" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="D349" s="4"/>
     </row>
@@ -7537,7 +7560,7 @@
         <v/>
       </c>
       <c r="C350" s="4" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="D350" s="4"/>
     </row>
@@ -7547,7 +7570,7 @@
         <v/>
       </c>
       <c r="C351" s="4" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="D351" s="4"/>
     </row>
@@ -7557,7 +7580,7 @@
         <v/>
       </c>
       <c r="C352" s="4" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="D352" s="4"/>
     </row>
@@ -7567,7 +7590,7 @@
         <v/>
       </c>
       <c r="C353" s="4" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="D353" s="4"/>
     </row>
@@ -7577,7 +7600,7 @@
         <v/>
       </c>
       <c r="C354" s="4" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="D354" s="4"/>
     </row>
@@ -7587,7 +7610,7 @@
         <v/>
       </c>
       <c r="C355" s="4" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="D355" s="4"/>
     </row>
@@ -7597,7 +7620,7 @@
         <v/>
       </c>
       <c r="C356" s="4" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="D356" s="4"/>
     </row>
@@ -7607,7 +7630,7 @@
         <v/>
       </c>
       <c r="C357" s="4" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="D357" s="4"/>
     </row>
@@ -7617,7 +7640,7 @@
         <v/>
       </c>
       <c r="C358" s="4" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="D358" s="4"/>
     </row>
@@ -7627,7 +7650,7 @@
         <v/>
       </c>
       <c r="C359" s="4" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D359" s="4"/>
     </row>
@@ -7647,7 +7670,7 @@
         <v/>
       </c>
       <c r="C361" s="4" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="D361" s="4"/>
     </row>
@@ -7677,7 +7700,7 @@
         <v/>
       </c>
       <c r="C364" s="4" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="D364" s="4"/>
     </row>
@@ -7687,7 +7710,7 @@
         <v/>
       </c>
       <c r="C365" s="4" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="D365" s="4"/>
     </row>
@@ -7707,7 +7730,7 @@
         <v/>
       </c>
       <c r="C367" s="4" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="D367" s="4"/>
     </row>
@@ -7717,7 +7740,7 @@
         <v>INFO</v>
       </c>
       <c r="C368" s="4" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="D368" s="4"/>
     </row>
@@ -7727,7 +7750,7 @@
         <v>INFO</v>
       </c>
       <c r="C369" s="4" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="D369" s="4"/>
     </row>
@@ -7797,7 +7820,7 @@
         <v/>
       </c>
       <c r="C376" s="4" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="D376" s="4"/>
     </row>
@@ -7835,7 +7858,7 @@
         <v/>
       </c>
       <c r="C380" s="4" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="D380" s="4"/>
     </row>
@@ -7855,7 +7878,7 @@
         <v/>
       </c>
       <c r="C382" s="4" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D382" s="4"/>
     </row>
@@ -7875,7 +7898,7 @@
         <v/>
       </c>
       <c r="C384" s="4" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D384" s="4"/>
     </row>
@@ -7885,7 +7908,7 @@
         <v>INFO</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="D385" s="4"/>
     </row>
@@ -7895,7 +7918,7 @@
         <v>INFO</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D386" s="4"/>
     </row>
@@ -7955,7 +7978,7 @@
         <v/>
       </c>
       <c r="C392" s="4" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="D392" s="4"/>
     </row>
@@ -8101,7 +8124,7 @@
         <v/>
       </c>
       <c r="C407" s="4" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D407" s="4"/>
     </row>
@@ -8129,7 +8152,7 @@
         <v/>
       </c>
       <c r="C410" s="4" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D410" s="4"/>
     </row>
@@ -8147,7 +8170,7 @@
         <v/>
       </c>
       <c r="C412" s="4" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D412" s="4"/>
     </row>
@@ -8211,7 +8234,7 @@
         <v/>
       </c>
       <c r="C419" s="4" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D419" s="4"/>
     </row>
@@ -8229,7 +8252,7 @@
         <v/>
       </c>
       <c r="C421" s="4" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D421" s="4"/>
     </row>
@@ -8257,7 +8280,7 @@
         <v/>
       </c>
       <c r="C424" s="4" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D424" s="4"/>
     </row>
@@ -8275,7 +8298,7 @@
         <v/>
       </c>
       <c r="C426" s="4" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D426" s="4"/>
     </row>
@@ -8285,7 +8308,7 @@
         <v/>
       </c>
       <c r="C427" s="4" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="D427" s="4"/>
     </row>
@@ -8303,7 +8326,7 @@
         <v/>
       </c>
       <c r="C429" s="4" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D429" s="4"/>
     </row>
@@ -8349,7 +8372,7 @@
         <v/>
       </c>
       <c r="C434" s="4" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="D434" s="4"/>
     </row>
@@ -8367,7 +8390,7 @@
         <v/>
       </c>
       <c r="C436" s="4" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D436" s="4"/>
     </row>
@@ -8395,7 +8418,7 @@
         <v/>
       </c>
       <c r="C439" s="4" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="D439" s="4"/>
     </row>
@@ -8413,7 +8436,7 @@
         <v/>
       </c>
       <c r="C441" s="4" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D441" s="4"/>
     </row>
@@ -8423,7 +8446,7 @@
         <v/>
       </c>
       <c r="C442" s="4" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="D442" s="4"/>
     </row>
@@ -8441,7 +8464,7 @@
         <v/>
       </c>
       <c r="C444" s="4" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D444" s="4"/>
     </row>
@@ -8509,7 +8532,7 @@
         <v/>
       </c>
       <c r="C451" s="4" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="D451" s="4"/>
     </row>
@@ -8527,7 +8550,7 @@
         <v/>
       </c>
       <c r="C453" s="4" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="D453" s="4"/>
     </row>
@@ -8537,7 +8560,7 @@
         <v/>
       </c>
       <c r="C454" s="4" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="D454" s="4"/>
     </row>
@@ -8585,7 +8608,7 @@
         <v/>
       </c>
       <c r="C459" s="4" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D459" s="4"/>
     </row>
@@ -8603,7 +8626,7 @@
         <v/>
       </c>
       <c r="C461" s="4" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D461" s="4"/>
     </row>
@@ -8613,7 +8636,7 @@
         <v/>
       </c>
       <c r="C462" s="4" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="D462" s="4"/>
     </row>
@@ -8661,7 +8684,7 @@
         <v/>
       </c>
       <c r="C467" s="4" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="D467" s="4"/>
     </row>
@@ -8671,7 +8694,7 @@
         <v/>
       </c>
       <c r="C468" s="4" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="D468" s="4"/>
     </row>
@@ -8689,7 +8712,7 @@
         <v/>
       </c>
       <c r="C470" s="4" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="D470" s="4"/>
     </row>
@@ -8699,7 +8722,7 @@
         <v/>
       </c>
       <c r="C471" s="4" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D471" s="4"/>
     </row>
@@ -8737,7 +8760,7 @@
         <v/>
       </c>
       <c r="C475" s="4" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="D475" s="4"/>
     </row>
@@ -8755,7 +8778,7 @@
         <v/>
       </c>
       <c r="C477" s="4" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="D477" s="4"/>
     </row>
@@ -8765,7 +8788,7 @@
         <v/>
       </c>
       <c r="C478" s="4" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="D478" s="4"/>
     </row>
@@ -8813,7 +8836,7 @@
         <v/>
       </c>
       <c r="C483" s="4" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="D483" s="4"/>
     </row>
@@ -8831,7 +8854,7 @@
         <v/>
       </c>
       <c r="C485" s="4" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D485" s="4"/>
     </row>
@@ -8841,7 +8864,7 @@
         <v/>
       </c>
       <c r="C486" s="4" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="D486" s="4"/>
     </row>
@@ -8879,7 +8902,7 @@
         <v/>
       </c>
       <c r="C490" s="4" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="D490" s="4"/>
     </row>
@@ -8897,7 +8920,7 @@
         <v/>
       </c>
       <c r="C492" s="4" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="D492" s="4"/>
     </row>
@@ -8907,7 +8930,7 @@
         <v/>
       </c>
       <c r="C493" s="4" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="D493" s="4"/>
     </row>
@@ -8963,7 +8986,7 @@
         <v/>
       </c>
       <c r="C499" s="4" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="D499" s="4"/>
     </row>
@@ -8981,7 +9004,7 @@
         <v/>
       </c>
       <c r="C501" s="4" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="D501" s="4"/>
     </row>
@@ -9035,7 +9058,7 @@
         <v/>
       </c>
       <c r="C507" s="4" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D507" s="4"/>
     </row>
@@ -9045,7 +9068,7 @@
         <v/>
       </c>
       <c r="C508" s="4" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="D508" s="4"/>
     </row>
@@ -9063,7 +9086,7 @@
         <v/>
       </c>
       <c r="C510" s="4" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="D510" s="4"/>
     </row>
@@ -9073,7 +9096,7 @@
         <v/>
       </c>
       <c r="C511" s="4" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="D511" s="4"/>
     </row>
@@ -9091,7 +9114,7 @@
         <v/>
       </c>
       <c r="C513" s="4" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="D513" s="4"/>
     </row>
@@ -9253,7 +9276,7 @@
         <v/>
       </c>
       <c r="C530" s="4" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="D530" s="4"/>
     </row>
@@ -9271,7 +9294,7 @@
         <v/>
       </c>
       <c r="C532" s="4" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="D532" s="4"/>
     </row>
@@ -9309,7 +9332,7 @@
         <v/>
       </c>
       <c r="C536" s="4" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="D536" s="4"/>
     </row>
@@ -9327,7 +9350,7 @@
         <v/>
       </c>
       <c r="C538" s="4" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="D538" s="4"/>
     </row>
@@ -9355,7 +9378,7 @@
         <v/>
       </c>
       <c r="C541" s="4" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D541" s="4"/>
     </row>
@@ -9373,7 +9396,7 @@
         <v/>
       </c>
       <c r="C543" s="4" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="D543" s="4"/>
     </row>
@@ -9401,7 +9424,7 @@
         <v/>
       </c>
       <c r="C546" s="4" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="D546" s="4"/>
     </row>
@@ -9411,7 +9434,7 @@
         <v/>
       </c>
       <c r="C547" s="4" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="D547" s="4"/>
     </row>
@@ -9429,7 +9452,7 @@
         <v/>
       </c>
       <c r="C549" s="4" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="D549" s="4"/>
     </row>
@@ -9663,7 +9686,7 @@
         <v/>
       </c>
       <c r="C573" s="4" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="D573" s="4"/>
     </row>
@@ -9673,7 +9696,7 @@
         <v/>
       </c>
       <c r="C574" s="4" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D574" s="4"/>
     </row>
@@ -9691,7 +9714,7 @@
         <v/>
       </c>
       <c r="C576" s="4" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="D576" s="4"/>
     </row>
@@ -9701,7 +9724,7 @@
         <v/>
       </c>
       <c r="C577" s="4" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="D577" s="4"/>
     </row>
@@ -9739,7 +9762,7 @@
         <v/>
       </c>
       <c r="C581" s="4" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="D581" s="4"/>
     </row>
@@ -9757,7 +9780,7 @@
         <v/>
       </c>
       <c r="C583" s="4" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="D583" s="4"/>
     </row>
@@ -9785,7 +9808,7 @@
         <v/>
       </c>
       <c r="C586" s="4" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="D586" s="4"/>
     </row>
@@ -9803,7 +9826,7 @@
         <v/>
       </c>
       <c r="C588" s="4" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="D588" s="4"/>
     </row>
@@ -9831,7 +9854,7 @@
         <v/>
       </c>
       <c r="C591" s="4" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="D591" s="4"/>
     </row>
@@ -9849,7 +9872,7 @@
         <v/>
       </c>
       <c r="C593" s="4" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="D593" s="4"/>
     </row>
@@ -9859,7 +9882,7 @@
         <v/>
       </c>
       <c r="C594" s="4" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="D594" s="4"/>
     </row>
@@ -9877,7 +9900,7 @@
         <v/>
       </c>
       <c r="C596" s="4" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="D596" s="4"/>
     </row>
@@ -9923,7 +9946,7 @@
         <v/>
       </c>
       <c r="C601" s="4" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="D601" s="4"/>
     </row>
@@ -9941,7 +9964,7 @@
         <v/>
       </c>
       <c r="C603" s="4" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="D603" s="4"/>
     </row>
@@ -9969,7 +9992,7 @@
         <v/>
       </c>
       <c r="C606" s="4" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="D606" s="4"/>
     </row>
@@ -9987,7 +10010,7 @@
         <v/>
       </c>
       <c r="C608" s="4" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="D608" s="4"/>
     </row>
@@ -10015,7 +10038,7 @@
         <v/>
       </c>
       <c r="C611" s="4" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="D611" s="4"/>
     </row>
@@ -10033,7 +10056,7 @@
         <v/>
       </c>
       <c r="C613" s="4" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="D613" s="4"/>
     </row>
@@ -10061,7 +10084,7 @@
         <v/>
       </c>
       <c r="C616" s="4" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="D616" s="4"/>
     </row>
@@ -10079,7 +10102,7 @@
         <v/>
       </c>
       <c r="C618" s="4" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="D618" s="4"/>
     </row>
@@ -10125,7 +10148,7 @@
         <v/>
       </c>
       <c r="C623" s="4" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="D623" s="4"/>
     </row>
@@ -10143,7 +10166,7 @@
         <v/>
       </c>
       <c r="C625" s="4" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="D625" s="4"/>
     </row>
@@ -10301,7 +10324,7 @@
         <v/>
       </c>
       <c r="C641" s="4" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="D641" s="4"/>
     </row>
@@ -10511,7 +10534,7 @@
         <v/>
       </c>
       <c r="C663" s="4" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="D663" s="4"/>
     </row>
@@ -10529,7 +10552,7 @@
         <v/>
       </c>
       <c r="C665" s="4" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D665" s="4"/>
     </row>
@@ -10539,7 +10562,7 @@
         <v/>
       </c>
       <c r="C666" s="4" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="D666" s="4"/>
     </row>
@@ -10557,7 +10580,7 @@
         <v/>
       </c>
       <c r="C668" s="4" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="D668" s="4"/>
     </row>
@@ -10567,7 +10590,7 @@
         <v/>
       </c>
       <c r="C669" s="4" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="D669" s="4"/>
     </row>
@@ -10585,7 +10608,7 @@
         <v/>
       </c>
       <c r="C671" s="4" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="D671" s="4"/>
     </row>
@@ -10631,7 +10654,7 @@
         <v/>
       </c>
       <c r="C676" s="4" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="D676" s="4"/>
     </row>
@@ -10649,7 +10672,7 @@
         <v/>
       </c>
       <c r="C678" s="4" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="D678" s="4"/>
     </row>
@@ -10677,7 +10700,7 @@
         <v/>
       </c>
       <c r="C681" s="4" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="D681" s="4"/>
     </row>
@@ -10695,7 +10718,7 @@
         <v/>
       </c>
       <c r="C683" s="4" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="D683" s="4"/>
     </row>
@@ -10723,7 +10746,7 @@
         <v/>
       </c>
       <c r="C686" s="4" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D686" s="4"/>
     </row>
@@ -10741,7 +10764,7 @@
         <v/>
       </c>
       <c r="C688" s="4" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="D688" s="4"/>
     </row>
@@ -10769,7 +10792,7 @@
         <v/>
       </c>
       <c r="C691" s="4" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="D691" s="4"/>
     </row>
@@ -10787,7 +10810,7 @@
         <v/>
       </c>
       <c r="C693" s="4" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="D693" s="4"/>
     </row>
@@ -10815,7 +10838,7 @@
         <v/>
       </c>
       <c r="C696" s="4" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="D696" s="4"/>
     </row>
@@ -10833,7 +10856,7 @@
         <v/>
       </c>
       <c r="C698" s="4" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D698" s="4"/>
     </row>
@@ -10861,7 +10884,7 @@
         <v/>
       </c>
       <c r="C701" s="4" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="D701" s="4"/>
     </row>
@@ -10879,7 +10902,7 @@
         <v/>
       </c>
       <c r="C703" s="4" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D703" s="4"/>
     </row>
@@ -10907,7 +10930,7 @@
         <v/>
       </c>
       <c r="C706" s="4" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="D706" s="4"/>
     </row>
@@ -10925,7 +10948,7 @@
         <v/>
       </c>
       <c r="C708" s="4" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D708" s="4"/>
     </row>
@@ -10935,7 +10958,7 @@
         <v/>
       </c>
       <c r="C709" s="4" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="D709" s="4"/>
     </row>
@@ -10953,7 +10976,7 @@
         <v/>
       </c>
       <c r="C711" s="4" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D711" s="4"/>
     </row>
@@ -11027,7 +11050,7 @@
         <v/>
       </c>
       <c r="C719" s="4" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="D719" s="4"/>
     </row>
@@ -11101,7 +11124,7 @@
         <v>INFO</v>
       </c>
       <c r="C727" s="4" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="D727" s="4"/>
     </row>
@@ -11111,7 +11134,7 @@
         <v/>
       </c>
       <c r="C728" s="4" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="D728" s="4"/>
     </row>
@@ -11129,7 +11152,7 @@
         <v/>
       </c>
       <c r="C730" s="4" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="D730" s="4"/>
     </row>
@@ -11149,7 +11172,7 @@
         <v/>
       </c>
       <c r="C732" s="4" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="D732" s="4"/>
     </row>
@@ -11167,7 +11190,7 @@
         <v/>
       </c>
       <c r="C734" s="4" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="D734" s="4"/>
     </row>
@@ -11177,7 +11200,7 @@
         <v/>
       </c>
       <c r="C735" s="4" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="D735" s="4"/>
     </row>
@@ -11195,7 +11218,7 @@
         <v/>
       </c>
       <c r="C737" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D737" s="4"/>
     </row>
@@ -11223,7 +11246,7 @@
         <v>INFO</v>
       </c>
       <c r="C740" s="4" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="D740" s="4"/>
     </row>
@@ -11233,7 +11256,7 @@
         <v/>
       </c>
       <c r="C741" s="4" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="D741" s="4"/>
     </row>
@@ -11251,7 +11274,7 @@
         <v/>
       </c>
       <c r="C743" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D743" s="4"/>
     </row>
@@ -11269,7 +11292,7 @@
         <v/>
       </c>
       <c r="C745" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D745" s="4"/>
     </row>
@@ -11279,7 +11302,7 @@
         <v/>
       </c>
       <c r="C746" s="4" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="D746" s="4"/>
     </row>
@@ -11297,7 +11320,7 @@
         <v/>
       </c>
       <c r="C748" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D748" s="4"/>
     </row>
@@ -11325,7 +11348,7 @@
         <v/>
       </c>
       <c r="C751" s="4" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="D751" s="4"/>
     </row>
@@ -11343,7 +11366,7 @@
         <v/>
       </c>
       <c r="C753" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D753" s="4"/>
     </row>
@@ -11389,7 +11412,7 @@
         <v>INFO</v>
       </c>
       <c r="C758" s="4" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="D758" s="4"/>
     </row>
@@ -11527,7 +11550,7 @@
         <v/>
       </c>
       <c r="C772" s="4" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="D772" s="4"/>
     </row>
@@ -11545,7 +11568,7 @@
         <v/>
       </c>
       <c r="C774" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D774" s="4"/>
     </row>
@@ -11555,7 +11578,7 @@
         <v/>
       </c>
       <c r="C775" s="4" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="D775" s="4"/>
     </row>
@@ -11573,7 +11596,7 @@
         <v/>
       </c>
       <c r="C777" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D777" s="4"/>
     </row>
@@ -11601,7 +11624,7 @@
         <v/>
       </c>
       <c r="C780" s="4" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="D780" s="4"/>
     </row>
@@ -11619,7 +11642,7 @@
         <v/>
       </c>
       <c r="C782" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D782" s="4"/>
     </row>
@@ -11629,7 +11652,7 @@
         <v/>
       </c>
       <c r="C783" s="4" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="D783" s="4"/>
     </row>
@@ -11647,7 +11670,7 @@
         <v/>
       </c>
       <c r="C785" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D785" s="4"/>
     </row>
@@ -11657,7 +11680,7 @@
         <v/>
       </c>
       <c r="C786" s="4" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="D786" s="4"/>
     </row>
@@ -11675,7 +11698,7 @@
         <v/>
       </c>
       <c r="C788" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D788" s="4"/>
     </row>
@@ -11745,7 +11768,7 @@
         <v/>
       </c>
       <c r="C795" s="4" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="D795" s="4"/>
     </row>
@@ -11765,7 +11788,7 @@
         <v/>
       </c>
       <c r="C797" s="4" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="D797" s="4"/>
     </row>
@@ -11889,7 +11912,7 @@
         <v/>
       </c>
       <c r="C810" s="4" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="D810" s="4"/>
     </row>
@@ -11899,7 +11922,7 @@
         <v/>
       </c>
       <c r="C811" s="4" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="D811" s="4"/>
     </row>
@@ -11909,7 +11932,7 @@
         <v/>
       </c>
       <c r="C812" s="4" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="D812" s="4"/>
     </row>
@@ -11927,7 +11950,7 @@
         <v/>
       </c>
       <c r="C814" s="4" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="D814" s="4"/>
     </row>
@@ -11973,7 +11996,7 @@
         <v/>
       </c>
       <c r="C819" s="4" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="D819" s="4"/>
     </row>
@@ -11991,7 +12014,7 @@
         <v/>
       </c>
       <c r="C821" s="4" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="D821" s="4"/>
     </row>
@@ -12019,7 +12042,7 @@
         <v/>
       </c>
       <c r="C824" s="4" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="D824" s="4"/>
     </row>
@@ -12037,7 +12060,7 @@
         <v/>
       </c>
       <c r="C826" s="4" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="D826" s="4"/>
     </row>
@@ -12075,7 +12098,7 @@
         <v/>
       </c>
       <c r="C830" s="4" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="D830" s="4"/>
     </row>
@@ -12093,7 +12116,7 @@
         <v/>
       </c>
       <c r="C832" s="4" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="D832" s="4"/>
     </row>
@@ -12103,7 +12126,7 @@
         <v>INFO</v>
       </c>
       <c r="C833" s="4" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="D833" s="4"/>
     </row>
@@ -12139,7 +12162,7 @@
         <v/>
       </c>
       <c r="C837" s="4" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="D837" s="4"/>
     </row>
@@ -12157,7 +12180,7 @@
         <v/>
       </c>
       <c r="C839" s="4" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="D839" s="4"/>
     </row>
@@ -12235,7 +12258,7 @@
         <v/>
       </c>
       <c r="C847" s="4" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="D847" s="4"/>
     </row>
@@ -12255,7 +12278,7 @@
         <v/>
       </c>
       <c r="C849" s="4" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="D849" s="4"/>
     </row>
@@ -12293,7 +12316,7 @@
         <v/>
       </c>
       <c r="C853" s="4" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="D853" s="4"/>
     </row>
@@ -12311,7 +12334,7 @@
         <v/>
       </c>
       <c r="C855" s="4" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="D855" s="4"/>
     </row>
@@ -12339,7 +12362,7 @@
         <v/>
       </c>
       <c r="C858" s="4" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="D858" s="4"/>
     </row>
@@ -12357,7 +12380,7 @@
         <v/>
       </c>
       <c r="C860" s="4" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="D860" s="4"/>
     </row>
@@ -12403,7 +12426,7 @@
         <v/>
       </c>
       <c r="C865" s="4" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="D865" s="4"/>
     </row>
@@ -12421,7 +12444,7 @@
         <v/>
       </c>
       <c r="C867" s="4" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="D867" s="4"/>
     </row>
@@ -12431,7 +12454,7 @@
         <v/>
       </c>
       <c r="C868" s="4" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="D868" s="4"/>
     </row>
@@ -12449,7 +12472,7 @@
         <v/>
       </c>
       <c r="C870" s="4" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="D870" s="4"/>
     </row>
@@ -12495,7 +12518,7 @@
         <v/>
       </c>
       <c r="C875" s="4" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="D875" s="4"/>
     </row>
@@ -12515,7 +12538,7 @@
         <v>INFO</v>
       </c>
       <c r="C877" s="4" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="D877" s="4"/>
     </row>
@@ -12533,7 +12556,7 @@
         <v/>
       </c>
       <c r="C879" s="4" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="D879" s="4"/>
     </row>
@@ -12551,7 +12574,7 @@
         <v/>
       </c>
       <c r="C881" s="4" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="D881" s="4"/>
     </row>
@@ -12561,7 +12584,7 @@
         <v/>
       </c>
       <c r="C882" s="4" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="D882" s="4"/>
     </row>
@@ -12579,7 +12602,7 @@
         <v/>
       </c>
       <c r="C884" s="4" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="D884" s="4"/>
     </row>
@@ -12643,7 +12666,7 @@
         <v/>
       </c>
       <c r="C891" s="4" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="D891" s="4"/>
     </row>
@@ -12661,7 +12684,7 @@
         <v/>
       </c>
       <c r="C893" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D893" s="4"/>
     </row>
@@ -12671,7 +12694,7 @@
         <v>INFO</v>
       </c>
       <c r="C894" s="4" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="D894" s="4"/>
     </row>
@@ -12689,7 +12712,7 @@
         <v/>
       </c>
       <c r="C896" s="4" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="D896" s="4"/>
     </row>
@@ -12707,7 +12730,7 @@
         <v/>
       </c>
       <c r="C898" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D898" s="4"/>
     </row>
@@ -12735,7 +12758,7 @@
         <v/>
       </c>
       <c r="C901" s="4" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="D901" s="4"/>
     </row>
@@ -12753,7 +12776,7 @@
         <v/>
       </c>
       <c r="C903" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D903" s="4"/>
     </row>
@@ -12763,7 +12786,7 @@
         <v/>
       </c>
       <c r="C904" s="4" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="D904" s="4"/>
     </row>
@@ -12781,7 +12804,7 @@
         <v/>
       </c>
       <c r="C906" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D906" s="4"/>
     </row>
@@ -12827,7 +12850,7 @@
         <v>INFO</v>
       </c>
       <c r="C911" s="4" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="D911" s="4"/>
     </row>
@@ -12845,7 +12868,7 @@
         <v/>
       </c>
       <c r="C913" s="4" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="D913" s="4"/>
     </row>
@@ -12863,7 +12886,7 @@
         <v/>
       </c>
       <c r="C915" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D915" s="4"/>
     </row>
@@ -12873,7 +12896,7 @@
         <v/>
       </c>
       <c r="C916" s="4" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="D916" s="4"/>
     </row>
@@ -12891,7 +12914,7 @@
         <v/>
       </c>
       <c r="C918" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D918" s="4"/>
     </row>
@@ -12937,7 +12960,7 @@
         <v/>
       </c>
       <c r="C923" s="4" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="D923" s="4"/>
     </row>
@@ -12947,7 +12970,7 @@
         <v/>
       </c>
       <c r="C924" s="4" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="D924" s="4"/>
     </row>
@@ -13045,7 +13068,7 @@
         <v/>
       </c>
       <c r="C934" s="4" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="D934" s="4"/>
     </row>
@@ -13063,7 +13086,7 @@
         <v/>
       </c>
       <c r="C936" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D936" s="4"/>
     </row>
@@ -13109,7 +13132,7 @@
         <v/>
       </c>
       <c r="C941" s="4" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="D941" s="4"/>
     </row>
@@ -13127,7 +13150,7 @@
         <v/>
       </c>
       <c r="C943" s="4" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D943" s="4"/>
     </row>
@@ -13155,7 +13178,7 @@
         <v/>
       </c>
       <c r="C946" s="4" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="D946" s="4"/>
     </row>
@@ -13173,7 +13196,7 @@
         <v/>
       </c>
       <c r="C948" s="4" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D948" s="4"/>
     </row>
@@ -13201,7 +13224,7 @@
         <v/>
       </c>
       <c r="C951" s="4" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="D951" s="4"/>
     </row>
@@ -13219,7 +13242,7 @@
         <v/>
       </c>
       <c r="C953" s="4" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D953" s="4"/>
     </row>
@@ -13247,7 +13270,7 @@
         <v>INFO</v>
       </c>
       <c r="C956" s="4" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="D956" s="4"/>
     </row>
@@ -13275,7 +13298,7 @@
         <v/>
       </c>
       <c r="C959" s="4" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="D959" s="4"/>
     </row>
@@ -13293,7 +13316,7 @@
         <v/>
       </c>
       <c r="C961" s="4" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D961" s="4"/>
     </row>
@@ -13303,7 +13326,7 @@
         <v/>
       </c>
       <c r="C962" s="4" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="D962" s="4"/>
     </row>
@@ -13331,7 +13354,7 @@
         <v/>
       </c>
       <c r="C965" s="4" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="D965" s="4"/>
     </row>
@@ -13349,7 +13372,7 @@
         <v/>
       </c>
       <c r="C967" s="4" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D967" s="4"/>
     </row>
@@ -13369,7 +13392,7 @@
         <v/>
       </c>
       <c r="C969" s="4" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="D969" s="4"/>
     </row>
@@ -13387,7 +13410,7 @@
         <v/>
       </c>
       <c r="C971" s="4" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D971" s="4"/>
     </row>
@@ -13445,7 +13468,7 @@
         <v/>
       </c>
       <c r="C977" s="4" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="D977" s="4"/>
     </row>
@@ -13495,7 +13518,7 @@
         <v>INFO</v>
       </c>
       <c r="C982" s="4" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="D982" s="4"/>
     </row>
@@ -13541,7 +13564,7 @@
         <v/>
       </c>
       <c r="C987" s="4" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="D987" s="4"/>
     </row>
@@ -13551,7 +13574,7 @@
         <v>INFO</v>
       </c>
       <c r="C988" s="4" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="D988" s="4"/>
     </row>
@@ -13807,7 +13830,7 @@
         <v/>
       </c>
       <c r="C1014" s="4" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="D1014" s="4"/>
     </row>
@@ -13817,7 +13840,7 @@
         <v/>
       </c>
       <c r="C1015" s="4" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="D1015" s="4"/>
     </row>
@@ -13827,7 +13850,7 @@
         <v/>
       </c>
       <c r="C1016" s="4" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="D1016" s="4"/>
     </row>
@@ -13837,7 +13860,7 @@
         <v/>
       </c>
       <c r="C1017" s="4" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="D1017" s="4"/>
     </row>
@@ -13847,7 +13870,7 @@
         <v/>
       </c>
       <c r="C1018" s="4" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="D1018" s="4"/>
     </row>
@@ -14801,7 +14824,7 @@
         <v/>
       </c>
       <c r="C1121" s="4" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="D1121" s="4"/>
     </row>
@@ -14811,7 +14834,7 @@
         <v/>
       </c>
       <c r="C1122" s="4" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="D1122" s="4"/>
     </row>
@@ -14821,7 +14844,7 @@
         <v/>
       </c>
       <c r="C1123" s="4" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="D1123" s="4"/>
     </row>
@@ -14941,7 +14964,7 @@
         <v/>
       </c>
       <c r="C1136" s="4" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="D1136" s="4"/>
     </row>
@@ -15015,7 +15038,7 @@
         <v/>
       </c>
       <c r="C1144" s="4" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="D1144" s="4"/>
     </row>
@@ -15025,7 +15048,7 @@
         <v/>
       </c>
       <c r="C1145" s="4" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="D1145" s="4"/>
     </row>
@@ -15035,7 +15058,7 @@
         <v/>
       </c>
       <c r="C1146" s="4" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="D1146" s="4"/>
     </row>
@@ -15109,7 +15132,7 @@
         <v/>
       </c>
       <c r="C1154" s="4" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="D1154" s="4"/>
     </row>
@@ -15119,7 +15142,7 @@
         <v/>
       </c>
       <c r="C1155" s="4" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="D1155" s="4"/>
     </row>
@@ -15193,7 +15216,7 @@
         <v/>
       </c>
       <c r="C1163" s="4" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="D1163" s="4"/>
     </row>
@@ -15203,7 +15226,7 @@
         <v/>
       </c>
       <c r="C1164" s="4" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="D1164" s="4"/>
     </row>
@@ -15637,7 +15660,7 @@
         <v/>
       </c>
       <c r="C1208" s="4" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="D1208" s="4"/>
     </row>
@@ -15697,7 +15720,7 @@
         <v>INFO</v>
       </c>
       <c r="C1214" s="4" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="D1214" s="4"/>
     </row>

</xml_diff>